<commit_message>
Better annealing and program to calculate route across licenses
Annealing now handles marked man and some stunt run events, and also
replaces events if it takes too long to travel to and from them. Also
created new program to take output of routes for single licenses and
output the total route + time
</commit_message>
<xml_diff>
--- a/map_data.xlsx
+++ b/map_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-3160" windowWidth="19200" windowHeight="19700" tabRatio="500"/>
+    <workbookView xWindow="28800" yWindow="-3160" windowWidth="19200" windowHeight="19680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="162">
   <si>
     <t>Avant Guard</t>
   </si>
@@ -212,6 +212,309 @@
   </si>
   <si>
     <t>junkyard</t>
+  </si>
+  <si>
+    <t>Emergency 911</t>
+  </si>
+  <si>
+    <t>2nd &amp; Hamilton</t>
+  </si>
+  <si>
+    <t>Club Sandwich</t>
+  </si>
+  <si>
+    <t>Evans &amp; 1st</t>
+  </si>
+  <si>
+    <t>Hostile Waters</t>
+  </si>
+  <si>
+    <t>Hall &amp; Manners</t>
+  </si>
+  <si>
+    <t>Mayday Mayday</t>
+  </si>
+  <si>
+    <t>Harber &amp; Manners</t>
+  </si>
+  <si>
+    <t>Power Struggle</t>
+  </si>
+  <si>
+    <t>2nd &amp; Fry</t>
+  </si>
+  <si>
+    <t>Press Ganged</t>
+  </si>
+  <si>
+    <t>I-88 Section 2 Tollbooth</t>
+  </si>
+  <si>
+    <t>Rescue Me</t>
+  </si>
+  <si>
+    <t>South Bay Expressway &amp; Parr</t>
+  </si>
+  <si>
+    <t>Run Home</t>
+  </si>
+  <si>
+    <t>West Lake &amp; Chubb</t>
+  </si>
+  <si>
+    <t>Run Like the Wind</t>
+  </si>
+  <si>
+    <t>Paradise &amp; 5th</t>
+  </si>
+  <si>
+    <t>Run to the Hills</t>
+  </si>
+  <si>
+    <t>King &amp; 3rd</t>
+  </si>
+  <si>
+    <t>Safe Harbor</t>
+  </si>
+  <si>
+    <t>Watt &amp; Angus</t>
+  </si>
+  <si>
+    <t>Seeing Stars</t>
+  </si>
+  <si>
+    <t>East Crawford &amp; Sullivan</t>
+  </si>
+  <si>
+    <t>Stampede</t>
+  </si>
+  <si>
+    <t>3rd &amp; Webster</t>
+  </si>
+  <si>
+    <t>Steeplechased</t>
+  </si>
+  <si>
+    <t>4th &amp; Root</t>
+  </si>
+  <si>
+    <t>Strike Out</t>
+  </si>
+  <si>
+    <t>Hamilton &amp; 5th</t>
+  </si>
+  <si>
+    <t>Marked Man</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>1st Street &amp; Hamilton Avenue</t>
+  </si>
+  <si>
+    <t>North Rouse Road &amp; Lewis Pass</t>
+  </si>
+  <si>
+    <t>Nelson Way &amp; Lucas Way</t>
+  </si>
+  <si>
+    <t>South Bay Expressway &amp; Hall Avenue</t>
+  </si>
+  <si>
+    <t>Warren Avenue &amp; Manners Avenue</t>
+  </si>
+  <si>
+    <t>Lambert Parkway &amp; East Crawford Drive</t>
+  </si>
+  <si>
+    <t>East Crawford Drive &amp; Hudson Avenue</t>
+  </si>
+  <si>
+    <t>East Lake Drive &amp; Ross Drive</t>
+  </si>
+  <si>
+    <t>West Lake Drive &amp; Nelson Way</t>
+  </si>
+  <si>
+    <t>Lucas Way &amp; Schembri Pass</t>
+  </si>
+  <si>
+    <t>2nd Street &amp; Root Avenue</t>
+  </si>
+  <si>
+    <t>3rd Street &amp; Hamilton Avenue</t>
+  </si>
+  <si>
+    <t>Nelson Way &amp; Chubb lane</t>
+  </si>
+  <si>
+    <t>Newton Drive &amp; West Crawford Drive</t>
+  </si>
+  <si>
+    <t>Nelson Way &amp; Lewis Pass</t>
+  </si>
+  <si>
+    <t>North Rouse Drive &amp; Read Lane</t>
+  </si>
+  <si>
+    <t>Gabriel Avenue &amp; Manners Avenue</t>
+  </si>
+  <si>
+    <t>South Mountain Drive &amp; Lucas Way</t>
+  </si>
+  <si>
+    <t>9th Street &amp; Hudson Avenue</t>
+  </si>
+  <si>
+    <t>Nelson Way &amp; East Lake Drive</t>
+  </si>
+  <si>
+    <t>3rd Street &amp; Angus Wharf</t>
+  </si>
+  <si>
+    <t>South Mountain Drive &amp; Schembri Pass</t>
+  </si>
+  <si>
+    <t>East Crawford Drive &amp; Moore Avenue</t>
+  </si>
+  <si>
+    <t>Cannon Pass &amp; Nelson Way</t>
+  </si>
+  <si>
+    <t>Lambert Parkway &amp; Harber Street</t>
+  </si>
+  <si>
+    <t>Hans Way &amp; West Lake Drive</t>
+  </si>
+  <si>
+    <t>South Rouse Drive &amp; South Bay Expressway</t>
+  </si>
+  <si>
+    <t>Franke Avenue &amp; Young Avenue</t>
+  </si>
+  <si>
+    <t>2nd Street &amp; Webster Avenue</t>
+  </si>
+  <si>
+    <t>South Rouse Drive &amp; Lambert Parkway</t>
+  </si>
+  <si>
+    <t>Andersen Street &amp; Glancey Avenue</t>
+  </si>
+  <si>
+    <t>Harber Street &amp; Hubbard Avenue</t>
+  </si>
+  <si>
+    <t>West Crawford Drive &amp; Nelson Way</t>
+  </si>
+  <si>
+    <t>Harber Street &amp; Glancey Avenue</t>
+  </si>
+  <si>
+    <t>1st Street &amp; Glancey Avenue</t>
+  </si>
+  <si>
+    <t>7th Street &amp; Webster Avenue</t>
+  </si>
+  <si>
+    <t>7th Street &amp; Hamilton Avenue</t>
+  </si>
+  <si>
+    <t>North Mountain Drive &amp; Hans Way</t>
+  </si>
+  <si>
+    <t>7th Street &amp; Glancey Avenue</t>
+  </si>
+  <si>
+    <t>South Rouse Drive &amp; Hubbard Avenue</t>
+  </si>
+  <si>
+    <t>About Town</t>
+  </si>
+  <si>
+    <t>Base Jumper</t>
+  </si>
+  <si>
+    <t>Bravo, Encore!</t>
+  </si>
+  <si>
+    <t>Cliffhanger</t>
+  </si>
+  <si>
+    <t>Elevation</t>
+  </si>
+  <si>
+    <t>Express Yourself</t>
+  </si>
+  <si>
+    <t>Falling Down</t>
+  </si>
+  <si>
+    <t>Hang 10</t>
+  </si>
+  <si>
+    <t>Lighthouse Party</t>
+  </si>
+  <si>
+    <t>Near the Edge</t>
+  </si>
+  <si>
+    <t>Offroad Parking</t>
+  </si>
+  <si>
+    <t>Over Construction</t>
+  </si>
+  <si>
+    <t>Rack 'Em Up</t>
+  </si>
+  <si>
+    <t>Unconventional</t>
+  </si>
+  <si>
+    <t>Stunt Run</t>
+  </si>
+  <si>
+    <t>Chubb &amp; West Lake</t>
+  </si>
+  <si>
+    <t>South Rouse &amp; Ross</t>
+  </si>
+  <si>
+    <t>3rd &amp; Lambert</t>
+  </si>
+  <si>
+    <t>Chubb &amp; Hans</t>
+  </si>
+  <si>
+    <t>1st &amp; Root</t>
+  </si>
+  <si>
+    <t>South Mountain &amp; South Bay Expressway</t>
+  </si>
+  <si>
+    <t>North Mountain &amp; Uphill</t>
+  </si>
+  <si>
+    <t>Lambert Parkway &amp; 9th</t>
+  </si>
+  <si>
+    <t>Patterson &amp; 9th</t>
+  </si>
+  <si>
+    <t>Nelson &amp; Read</t>
+  </si>
+  <si>
+    <t>Lambert &amp; Hall</t>
+  </si>
+  <si>
+    <t>Harber &amp; Warren</t>
+  </si>
+  <si>
+    <t>East Lake &amp; Rack</t>
+  </si>
+  <si>
+    <t>Andersen &amp; Angus</t>
   </si>
 </sst>
 </file>
@@ -221,7 +524,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm:ss.0;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -246,12 +549,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -262,6 +559,18 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -286,12 +595,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -570,20 +881,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>58</v>
       </c>
@@ -596,12 +910,15 @@
       <c r="D1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2">
@@ -613,12 +930,15 @@
       <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -630,12 +950,15 @@
       <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
@@ -647,12 +970,15 @@
       <c r="D4" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B5">
@@ -664,12 +990,15 @@
       <c r="D5" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B6">
@@ -681,12 +1010,15 @@
       <c r="D6" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -698,12 +1030,15 @@
       <c r="D7" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -715,12 +1050,15 @@
       <c r="D8" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -732,12 +1070,15 @@
       <c r="D9" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -749,12 +1090,15 @@
       <c r="D10" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B11">
@@ -766,12 +1110,15 @@
       <c r="D11" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B12">
@@ -783,12 +1130,15 @@
       <c r="D12" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B13">
@@ -800,12 +1150,15 @@
       <c r="D13" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B14">
@@ -817,12 +1170,15 @@
       <c r="D14" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B15">
@@ -834,12 +1190,15 @@
       <c r="D15" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B16">
@@ -851,12 +1210,15 @@
       <c r="D16" t="s">
         <v>1</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B17">
@@ -868,12 +1230,15 @@
       <c r="D17" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B18">
@@ -885,12 +1250,15 @@
       <c r="D18" t="s">
         <v>1</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B19">
@@ -902,12 +1270,15 @@
       <c r="D19" t="s">
         <v>1</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B20">
@@ -919,12 +1290,15 @@
       <c r="D20" t="s">
         <v>1</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B21">
@@ -936,12 +1310,15 @@
       <c r="D21" t="s">
         <v>1</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B22">
@@ -953,12 +1330,15 @@
       <c r="D22" t="s">
         <v>1</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B23">
@@ -970,12 +1350,15 @@
       <c r="D23" t="s">
         <v>1</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B24">
@@ -987,12 +1370,15 @@
       <c r="D24" t="s">
         <v>1</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B25">
@@ -1004,12 +1390,15 @@
       <c r="D25" t="s">
         <v>1</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B26">
@@ -1021,12 +1410,15 @@
       <c r="D26" t="s">
         <v>1</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B27">
@@ -1038,12 +1430,15 @@
       <c r="D27" t="s">
         <v>1</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B28">
@@ -1055,12 +1450,15 @@
       <c r="D28" t="s">
         <v>1</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B29">
@@ -1072,12 +1470,15 @@
       <c r="D29" t="s">
         <v>1</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B30">
@@ -1089,12 +1490,15 @@
       <c r="D30" t="s">
         <v>1</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B31">
@@ -1106,12 +1510,15 @@
       <c r="D31" t="s">
         <v>1</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B32">
@@ -1123,12 +1530,15 @@
       <c r="D32" t="s">
         <v>1</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B33">
@@ -1140,12 +1550,15 @@
       <c r="D33" t="s">
         <v>1</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B34">
@@ -1157,12 +1570,15 @@
       <c r="D34" t="s">
         <v>1</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B35">
@@ -1174,110 +1590,696 @@
       <c r="D35" t="s">
         <v>1</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="3">
         <v>1468</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="3">
         <v>814</v>
       </c>
       <c r="D36" t="s">
         <v>1</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F36" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="3">
         <v>1496</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="3">
         <v>468</v>
       </c>
       <c r="D37" t="s">
         <v>1</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F37" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="3">
         <v>1159</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="3">
         <v>457</v>
       </c>
       <c r="D38" t="s">
         <v>1</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E38" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="3">
         <v>210</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="3">
         <v>892</v>
       </c>
       <c r="D39" t="s">
         <v>1</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E39" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F39" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="3">
         <v>1450</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="3">
         <v>485</v>
       </c>
       <c r="D40" t="s">
         <v>1</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E40" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F40" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="3">
         <v>867</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="3">
         <v>805</v>
       </c>
       <c r="D41" t="s">
         <v>1</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E41" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F41" s="3" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" s="3">
+        <v>1214</v>
+      </c>
+      <c r="C42" s="3">
+        <v>801</v>
+      </c>
+      <c r="D42" t="s">
+        <v>91</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B43" s="3">
+        <v>1160</v>
+      </c>
+      <c r="C43" s="3">
+        <v>730</v>
+      </c>
+      <c r="D43" t="s">
+        <v>91</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" s="3">
+        <v>912</v>
+      </c>
+      <c r="C44" s="3">
+        <v>975</v>
+      </c>
+      <c r="D44" t="s">
+        <v>91</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" s="5">
+        <v>1205</v>
+      </c>
+      <c r="C45" s="3">
+        <v>866</v>
+      </c>
+      <c r="D45" t="s">
+        <v>91</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B46" s="5">
+        <v>1286</v>
+      </c>
+      <c r="C46" s="3">
+        <v>737</v>
+      </c>
+      <c r="D46" t="s">
+        <v>91</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="5">
+        <v>1521</v>
+      </c>
+      <c r="C47" s="3">
+        <v>526</v>
+      </c>
+      <c r="D47" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B48" s="5">
+        <v>1015</v>
+      </c>
+      <c r="C48" s="3">
+        <v>1067</v>
+      </c>
+      <c r="D48" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B49" s="5">
+        <v>396</v>
+      </c>
+      <c r="C49" s="3">
+        <v>689</v>
+      </c>
+      <c r="D49" t="s">
+        <v>91</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" s="5">
+        <v>1310</v>
+      </c>
+      <c r="C50" s="3">
+        <v>598</v>
+      </c>
+      <c r="D50" t="s">
+        <v>91</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B51" s="5">
+        <v>1262</v>
+      </c>
+      <c r="C51" s="3">
+        <v>671</v>
+      </c>
+      <c r="D51" t="s">
+        <v>91</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B52" s="5">
+        <v>1582</v>
+      </c>
+      <c r="C52" s="3">
+        <v>477</v>
+      </c>
+      <c r="D52" t="s">
+        <v>91</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B53" s="5">
+        <v>1226</v>
+      </c>
+      <c r="C53" s="3">
+        <v>340</v>
+      </c>
+      <c r="D53" t="s">
+        <v>91</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B54" s="5">
+        <v>1511</v>
+      </c>
+      <c r="C54" s="3">
+        <v>697</v>
+      </c>
+      <c r="D54" t="s">
+        <v>91</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B55" s="5">
+        <v>1372</v>
+      </c>
+      <c r="C55" s="3">
+        <v>636</v>
+      </c>
+      <c r="D55" t="s">
+        <v>91</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B56" s="5">
+        <v>1149</v>
+      </c>
+      <c r="C56" s="3">
+        <v>560</v>
+      </c>
+      <c r="D56" t="s">
+        <v>91</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B57" s="3">
+        <v>314</v>
+      </c>
+      <c r="C57" s="3">
+        <v>469</v>
+      </c>
+      <c r="D57" t="s">
+        <v>147</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B58" s="3">
+        <v>802</v>
+      </c>
+      <c r="C58" s="3">
+        <v>464</v>
+      </c>
+      <c r="D58" t="s">
+        <v>147</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B59" s="3">
+        <v>1071</v>
+      </c>
+      <c r="C59" s="3">
+        <v>619</v>
+      </c>
+      <c r="D59" t="s">
+        <v>147</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B60" s="3">
+        <v>373</v>
+      </c>
+      <c r="C60" s="3">
+        <v>867</v>
+      </c>
+      <c r="D60" t="s">
+        <v>147</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F60" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B61" s="3">
+        <v>1377</v>
+      </c>
+      <c r="C61" s="3">
+        <v>803</v>
+      </c>
+      <c r="D61" t="s">
+        <v>147</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="F61" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B62" s="3">
+        <v>571</v>
+      </c>
+      <c r="C62" s="3">
+        <v>1077</v>
+      </c>
+      <c r="D62" t="s">
+        <v>147</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F62" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B63" s="3">
+        <v>120</v>
+      </c>
+      <c r="C63" s="3">
+        <v>467</v>
+      </c>
+      <c r="D63" t="s">
+        <v>147</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="F63" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B64" s="3">
+        <v>1091</v>
+      </c>
+      <c r="C64" s="3">
+        <v>400</v>
+      </c>
+      <c r="D64" t="s">
+        <v>147</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F64" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B65" s="3">
+        <v>1434</v>
+      </c>
+      <c r="C65" s="3">
+        <v>447</v>
+      </c>
+      <c r="D65" t="s">
+        <v>147</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F65" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B66" s="3">
+        <v>370</v>
+      </c>
+      <c r="C66" s="3">
+        <v>210</v>
+      </c>
+      <c r="D66" t="s">
+        <v>147</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B67" s="3">
+        <v>900</v>
+      </c>
+      <c r="C67" s="3">
+        <v>913</v>
+      </c>
+      <c r="D67" t="s">
+        <v>147</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F67" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B68" s="3">
+        <v>1109</v>
+      </c>
+      <c r="C68" s="3">
+        <v>867</v>
+      </c>
+      <c r="D68" t="s">
+        <v>147</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F68" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B69" s="3">
+        <v>636</v>
+      </c>
+      <c r="C69" s="3">
+        <v>586</v>
+      </c>
+      <c r="D69" t="s">
+        <v>147</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B70" s="3">
+        <v>1560</v>
+      </c>
+      <c r="C70" s="3">
+        <v>652</v>
+      </c>
+      <c r="D70" t="s">
+        <v>147</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F70" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1322,6 +2324,16 @@
     <hyperlink ref="A39" r:id="rId38" tooltip="Torpedo Run"/>
     <hyperlink ref="A40" r:id="rId39" tooltip="Tunnel Vision"/>
     <hyperlink ref="A41" r:id="rId40" tooltip="Waterway to Go"/>
+    <hyperlink ref="A42" r:id="rId41" tooltip="Club Sandwich"/>
+    <hyperlink ref="A49" r:id="rId42" tooltip="Run Home"/>
+    <hyperlink ref="A52" r:id="rId43" tooltip="Safe Harbor"/>
+    <hyperlink ref="A53" r:id="rId44" tooltip="Seeing Stars"/>
+    <hyperlink ref="A56" r:id="rId45" tooltip="Strike Out"/>
+    <hyperlink ref="A60" r:id="rId46" tooltip="Cliffhanger (Burnout Paradise)"/>
+    <hyperlink ref="A62" r:id="rId47" tooltip="Express Yourself"/>
+    <hyperlink ref="A63" r:id="rId48" tooltip="Falling Down (Burnout Paradise)"/>
+    <hyperlink ref="A64" r:id="rId49" tooltip="Hang 10"/>
+    <hyperlink ref="A68" r:id="rId50" tooltip="Over Construction"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>